<commit_message>
append url, move DC to top100 cities
</commit_message>
<xml_diff>
--- a/data/missing_county_2020_2021.xlsx
+++ b/data/missing_county_2020_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/state_county_city/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tn/Desktop/REASON/acfrs_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19D35DF8-17EF-604A-8BF0-B802D9752C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AC8A7BE5-E562-AD43-8640-4B1C07C3D5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7300" yWindow="500" windowWidth="37500" windowHeight="22980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3461,9 +3461,6 @@
     <t>https://www.essexma.org/sites/g/files/vyhlif4406/f/uploads/fy21_audit.pdf</t>
   </si>
   <si>
-    <t xml:space="preserve">only has MIDDLESEX COUNTY RETIREMENT SYSTEM </t>
-  </si>
-  <si>
     <t>https://middlesexretirement.org/wp-content/uploads/2021/08/Middlesex-Retirement-12-31-2020-Financial-Statements-FINAL.pdf</t>
   </si>
   <si>
@@ -3471,6 +3468,9 @@
   </si>
   <si>
     <t>https://www.nd.gov/auditor/counties#AgyW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middessex county was abolished in 1997, only has TOWN of ESSEX .only has MIDDLESEX COUNTY RETIREMENT SYSTEM </t>
   </si>
 </sst>
 </file>
@@ -4425,8 +4425,8 @@
   <dimension ref="A1:K1084"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A696" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J718" sqref="J718"/>
+      <pane ySplit="1" topLeftCell="A718" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K748" sqref="K748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6101,7 +6101,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="119" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="170" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>82</v>
       </c>
@@ -10037,7 +10037,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:11" ht="153" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>260</v>
       </c>
@@ -11349,7 +11349,7 @@
         <v>1094</v>
       </c>
     </row>
-    <row r="316" spans="1:11" ht="204" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:11" ht="272" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>322</v>
       </c>
@@ -14423,10 +14423,10 @@
         <v>8</v>
       </c>
       <c r="J450" t="s">
+        <v>1138</v>
+      </c>
+      <c r="K450" t="s">
         <v>1135</v>
-      </c>
-      <c r="K450" t="s">
-        <v>1136</v>
       </c>
     </row>
     <row r="451" spans="1:11" x14ac:dyDescent="0.2">
@@ -18332,10 +18332,10 @@
         <v>8</v>
       </c>
       <c r="J625" s="7" t="s">
+        <v>1136</v>
+      </c>
+      <c r="K625" t="s">
         <v>1137</v>
-      </c>
-      <c r="K625" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="626" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>